<commit_message>
getting the correct values
</commit_message>
<xml_diff>
--- a/assignment-2/compiled_invoices.xlsx
+++ b/assignment-2/compiled_invoices.xlsx
@@ -473,10 +473,10 @@
         <v>785.71</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>102.14</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>887.85</v>
       </c>
     </row>
     <row r="3">
@@ -492,10 +492,10 @@
         <v>3492.07</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>453.97</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>3946.04</v>
       </c>
     </row>
     <row r="4">
@@ -511,10 +511,10 @@
         <v>1713.66</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>222.78</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>1936.44</v>
       </c>
     </row>
     <row r="5">
@@ -530,10 +530,10 @@
         <v>4849.66</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>630.46</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>5480.12</v>
       </c>
     </row>
     <row r="6">
@@ -549,10 +549,10 @@
         <v>480.62</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>62.48</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>543.1</v>
       </c>
     </row>
     <row r="7">
@@ -568,10 +568,10 @@
         <v>887.47</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>115.37</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>1002.84</v>
       </c>
     </row>
     <row r="8">
@@ -587,10 +587,10 @@
         <v>617.29</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>80.25</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>697.54</v>
       </c>
     </row>
     <row r="9">
@@ -606,10 +606,10 @@
         <v>820.2</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>106.63</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>926.83</v>
       </c>
     </row>
     <row r="10">
@@ -625,10 +625,10 @@
         <v>2740.91</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>356.32</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>3097.23</v>
       </c>
     </row>
     <row r="11">
@@ -644,10 +644,10 @@
         <v>650.27</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>84.54000000000001</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>734.8099999999999</v>
       </c>
     </row>
     <row r="12">
@@ -663,10 +663,10 @@
         <v>524.5700000000001</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>68.19</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>592.76</v>
       </c>
     </row>
     <row r="13">
@@ -682,10 +682,10 @@
         <v>666.78</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>86.68000000000001</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>753.46</v>
       </c>
     </row>
     <row r="14">
@@ -701,10 +701,10 @@
         <v>9836.09</v>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>1278.69</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>11114.78</v>
       </c>
     </row>
     <row r="15">
@@ -720,10 +720,10 @@
         <v>1554.23</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>202.05</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>1756.28</v>
       </c>
     </row>
     <row r="16">
@@ -739,10 +739,10 @@
         <v>2927.2</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>380.54</v>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>3307.74</v>
       </c>
     </row>
     <row r="17">
@@ -758,10 +758,10 @@
         <v>514.72</v>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>66.91</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>581.63</v>
       </c>
     </row>
     <row r="18">
@@ -777,10 +777,10 @@
         <v>841.25</v>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>109.36</v>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>950.61</v>
       </c>
     </row>
     <row r="19">
@@ -796,10 +796,10 @@
         <v>436.1</v>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>56.69</v>
       </c>
       <c r="E19" t="n">
-        <v>0</v>
+        <v>492.79</v>
       </c>
     </row>
     <row r="20">
@@ -815,10 +815,10 @@
         <v>850.22</v>
       </c>
       <c r="D20" t="n">
-        <v>0</v>
+        <v>110.53</v>
       </c>
       <c r="E20" t="n">
-        <v>0</v>
+        <v>960.75</v>
       </c>
     </row>
     <row r="21">
@@ -834,10 +834,10 @@
         <v>6613.79</v>
       </c>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>859.79</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>7473.58</v>
       </c>
     </row>
     <row r="22">
@@ -853,10 +853,10 @@
         <v>1366.8</v>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>177.68</v>
       </c>
       <c r="E22" t="n">
-        <v>0</v>
+        <v>1544.48</v>
       </c>
     </row>
     <row r="23">
@@ -872,10 +872,10 @@
         <v>415.24</v>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>53.98</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>469.22</v>
       </c>
     </row>
     <row r="24">
@@ -891,10 +891,10 @@
         <v>6999.98</v>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>910</v>
       </c>
       <c r="E24" t="n">
-        <v>0</v>
+        <v>7909.98</v>
       </c>
     </row>
     <row r="25">
@@ -910,10 +910,10 @@
         <v>380.88</v>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>49.51</v>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>430.39</v>
       </c>
     </row>
     <row r="26">
@@ -929,10 +929,10 @@
         <v>4155.75</v>
       </c>
       <c r="D26" t="n">
-        <v>0</v>
+        <v>540.25</v>
       </c>
       <c r="E26" t="n">
-        <v>0</v>
+        <v>4696</v>
       </c>
     </row>
     <row r="27">
@@ -948,10 +948,10 @@
         <v>3785.59</v>
       </c>
       <c r="D27" t="n">
-        <v>0</v>
+        <v>492.13</v>
       </c>
       <c r="E27" t="n">
-        <v>0</v>
+        <v>4277.72</v>
       </c>
     </row>
     <row r="28">
@@ -967,10 +967,10 @@
         <v>502.77</v>
       </c>
       <c r="D28" t="n">
-        <v>0</v>
+        <v>65.36</v>
       </c>
       <c r="E28" t="n">
-        <v>0</v>
+        <v>568.13</v>
       </c>
     </row>
     <row r="29">
@@ -986,10 +986,10 @@
         <v>8079.6</v>
       </c>
       <c r="D29" t="n">
-        <v>0</v>
+        <v>1050.35</v>
       </c>
       <c r="E29" t="n">
-        <v>0</v>
+        <v>9129.950000000001</v>
       </c>
     </row>
     <row r="30">
@@ -1005,10 +1005,10 @@
         <v>308.19</v>
       </c>
       <c r="D30" t="n">
-        <v>0</v>
+        <v>40.06</v>
       </c>
       <c r="E30" t="n">
-        <v>0</v>
+        <v>348.25</v>
       </c>
     </row>
     <row r="31">
@@ -1024,10 +1024,10 @@
         <v>6316.75</v>
       </c>
       <c r="D31" t="n">
-        <v>0</v>
+        <v>821.1799999999999</v>
       </c>
       <c r="E31" t="n">
-        <v>0</v>
+        <v>7137.93</v>
       </c>
     </row>
     <row r="32">
@@ -1043,10 +1043,10 @@
         <v>477.04</v>
       </c>
       <c r="D32" t="n">
-        <v>0</v>
+        <v>62.02</v>
       </c>
       <c r="E32" t="n">
-        <v>0</v>
+        <v>539.0599999999999</v>
       </c>
     </row>
     <row r="33">
@@ -1062,10 +1062,10 @@
         <v>8497.059999999999</v>
       </c>
       <c r="D33" t="n">
-        <v>0</v>
+        <v>1104.62</v>
       </c>
       <c r="E33" t="n">
-        <v>0</v>
+        <v>9601.68</v>
       </c>
     </row>
     <row r="34">
@@ -1081,10 +1081,10 @@
         <v>1111.28</v>
       </c>
       <c r="D34" t="n">
-        <v>0</v>
+        <v>144.47</v>
       </c>
       <c r="E34" t="n">
-        <v>0</v>
+        <v>1255.75</v>
       </c>
     </row>
     <row r="35">
@@ -1100,10 +1100,10 @@
         <v>8501.700000000001</v>
       </c>
       <c r="D35" t="n">
-        <v>0</v>
+        <v>1105.22</v>
       </c>
       <c r="E35" t="n">
-        <v>0</v>
+        <v>9606.92</v>
       </c>
     </row>
     <row r="36">
@@ -1119,10 +1119,10 @@
         <v>3848.3</v>
       </c>
       <c r="D36" t="n">
-        <v>0</v>
+        <v>500.28</v>
       </c>
       <c r="E36" t="n">
-        <v>0</v>
+        <v>4348.58</v>
       </c>
     </row>
     <row r="37">
@@ -1138,10 +1138,10 @@
         <v>5048.34</v>
       </c>
       <c r="D37" t="n">
-        <v>0</v>
+        <v>656.28</v>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
+        <v>5704.62</v>
       </c>
     </row>
     <row r="38">
@@ -1157,10 +1157,10 @@
         <v>5077.89</v>
       </c>
       <c r="D38" t="n">
-        <v>0</v>
+        <v>660.13</v>
       </c>
       <c r="E38" t="n">
-        <v>0</v>
+        <v>5738.02</v>
       </c>
     </row>
     <row r="39">
@@ -1176,10 +1176,10 @@
         <v>203.02</v>
       </c>
       <c r="D39" t="n">
-        <v>0</v>
+        <v>26.39</v>
       </c>
       <c r="E39" t="n">
-        <v>0</v>
+        <v>229.41</v>
       </c>
     </row>
     <row r="40">
@@ -1195,10 +1195,10 @@
         <v>876.76</v>
       </c>
       <c r="D40" t="n">
-        <v>0</v>
+        <v>113.98</v>
       </c>
       <c r="E40" t="n">
-        <v>0</v>
+        <v>990.74</v>
       </c>
     </row>
     <row r="41">
@@ -1214,10 +1214,10 @@
         <v>881.58</v>
       </c>
       <c r="D41" t="n">
-        <v>0</v>
+        <v>114.61</v>
       </c>
       <c r="E41" t="n">
-        <v>0</v>
+        <v>996.1900000000001</v>
       </c>
     </row>
     <row r="42">
@@ -1233,10 +1233,10 @@
         <v>4579.85</v>
       </c>
       <c r="D42" t="n">
-        <v>0</v>
+        <v>595.38</v>
       </c>
       <c r="E42" t="n">
-        <v>0</v>
+        <v>5175.23</v>
       </c>
     </row>
     <row r="43">
@@ -1252,10 +1252,10 @@
         <v>7849.93</v>
       </c>
       <c r="D43" t="n">
-        <v>0</v>
+        <v>1020.49</v>
       </c>
       <c r="E43" t="n">
-        <v>0</v>
+        <v>8870.42</v>
       </c>
     </row>
     <row r="44">
@@ -1271,10 +1271,10 @@
         <v>6729.27</v>
       </c>
       <c r="D44" t="n">
-        <v>0</v>
+        <v>874.8099999999999</v>
       </c>
       <c r="E44" t="n">
-        <v>0</v>
+        <v>7604.08</v>
       </c>
     </row>
     <row r="45">
@@ -1290,10 +1290,10 @@
         <v>1394.89</v>
       </c>
       <c r="D45" t="n">
-        <v>0</v>
+        <v>181.34</v>
       </c>
       <c r="E45" t="n">
-        <v>0</v>
+        <v>1576.23</v>
       </c>
     </row>
     <row r="46">
@@ -1309,10 +1309,10 @@
         <v>641.3099999999999</v>
       </c>
       <c r="D46" t="n">
-        <v>0</v>
+        <v>83.37</v>
       </c>
       <c r="E46" t="n">
-        <v>0</v>
+        <v>724.6799999999999</v>
       </c>
     </row>
     <row r="47">
@@ -1328,10 +1328,10 @@
         <v>917.41</v>
       </c>
       <c r="D47" t="n">
-        <v>0</v>
+        <v>119.26</v>
       </c>
       <c r="E47" t="n">
-        <v>0</v>
+        <v>1036.67</v>
       </c>
     </row>
     <row r="48">
@@ -1347,10 +1347,10 @@
         <v>691.65</v>
       </c>
       <c r="D48" t="n">
-        <v>0</v>
+        <v>89.91</v>
       </c>
       <c r="E48" t="n">
-        <v>0</v>
+        <v>781.5599999999999</v>
       </c>
     </row>
     <row r="49">
@@ -1366,10 +1366,10 @@
         <v>2366.99</v>
       </c>
       <c r="D49" t="n">
-        <v>0</v>
+        <v>307.71</v>
       </c>
       <c r="E49" t="n">
-        <v>0</v>
+        <v>2674.7</v>
       </c>
     </row>
     <row r="50">
@@ -1385,10 +1385,10 @@
         <v>2684.19</v>
       </c>
       <c r="D50" t="n">
-        <v>0</v>
+        <v>348.94</v>
       </c>
       <c r="E50" t="n">
-        <v>0</v>
+        <v>3033.13</v>
       </c>
     </row>
     <row r="51">
@@ -1404,10 +1404,10 @@
         <v>644.2</v>
       </c>
       <c r="D51" t="n">
-        <v>0</v>
+        <v>83.75</v>
       </c>
       <c r="E51" t="n">
-        <v>0</v>
+        <v>727.95</v>
       </c>
     </row>
     <row r="52">
@@ -1423,10 +1423,10 @@
         <v>395.95</v>
       </c>
       <c r="D52" t="n">
-        <v>0</v>
+        <v>51.47</v>
       </c>
       <c r="E52" t="n">
-        <v>0</v>
+        <v>447.42</v>
       </c>
     </row>
     <row r="53">
@@ -1442,10 +1442,10 @@
         <v>6988.38</v>
       </c>
       <c r="D53" t="n">
-        <v>0</v>
+        <v>908.49</v>
       </c>
       <c r="E53" t="n">
-        <v>0</v>
+        <v>7896.87</v>
       </c>
     </row>
     <row r="54">
@@ -1461,10 +1461,10 @@
         <v>621.9400000000001</v>
       </c>
       <c r="D54" t="n">
-        <v>0</v>
+        <v>80.84999999999999</v>
       </c>
       <c r="E54" t="n">
-        <v>0</v>
+        <v>702.79</v>
       </c>
     </row>
     <row r="55">
@@ -1480,10 +1480,10 @@
         <v>6568.68</v>
       </c>
       <c r="D55" t="n">
-        <v>0</v>
+        <v>853.9299999999999</v>
       </c>
       <c r="E55" t="n">
-        <v>0</v>
+        <v>7422.61</v>
       </c>
     </row>
     <row r="56">
@@ -1499,10 +1499,10 @@
         <v>791.41</v>
       </c>
       <c r="D56" t="n">
-        <v>0</v>
+        <v>102.88</v>
       </c>
       <c r="E56" t="n">
-        <v>0</v>
+        <v>894.29</v>
       </c>
     </row>
     <row r="57">
@@ -1518,10 +1518,10 @@
         <v>4981.83</v>
       </c>
       <c r="D57" t="n">
-        <v>0</v>
+        <v>647.64</v>
       </c>
       <c r="E57" t="n">
-        <v>0</v>
+        <v>5629.47</v>
       </c>
     </row>
     <row r="58">
@@ -1537,10 +1537,10 @@
         <v>168.11</v>
       </c>
       <c r="D58" t="n">
-        <v>0</v>
+        <v>21.85</v>
       </c>
       <c r="E58" t="n">
-        <v>0</v>
+        <v>189.96</v>
       </c>
     </row>
     <row r="59">
@@ -1556,10 +1556,10 @@
         <v>1141.49</v>
       </c>
       <c r="D59" t="n">
-        <v>0</v>
+        <v>148.39</v>
       </c>
       <c r="E59" t="n">
-        <v>0</v>
+        <v>1289.88</v>
       </c>
     </row>
     <row r="60">
@@ -1575,10 +1575,10 @@
         <v>5668.66</v>
       </c>
       <c r="D60" t="n">
-        <v>0</v>
+        <v>736.9299999999999</v>
       </c>
       <c r="E60" t="n">
-        <v>0</v>
+        <v>6405.59</v>
       </c>
     </row>
     <row r="61">
@@ -1594,10 +1594,10 @@
         <v>918.2</v>
       </c>
       <c r="D61" t="n">
-        <v>0</v>
+        <v>119.37</v>
       </c>
       <c r="E61" t="n">
-        <v>0</v>
+        <v>1037.57</v>
       </c>
     </row>
     <row r="62">
@@ -1613,10 +1613,10 @@
         <v>6581.29</v>
       </c>
       <c r="D62" t="n">
-        <v>0</v>
+        <v>855.5700000000001</v>
       </c>
       <c r="E62" t="n">
-        <v>0</v>
+        <v>7436.86</v>
       </c>
     </row>
     <row r="63">
@@ -1632,10 +1632,10 @@
         <v>196.76</v>
       </c>
       <c r="D63" t="n">
-        <v>0</v>
+        <v>25.58</v>
       </c>
       <c r="E63" t="n">
-        <v>0</v>
+        <v>222.34</v>
       </c>
     </row>
     <row r="64">
@@ -1651,10 +1651,10 @@
         <v>2303.03</v>
       </c>
       <c r="D64" t="n">
-        <v>0</v>
+        <v>299.39</v>
       </c>
       <c r="E64" t="n">
-        <v>0</v>
+        <v>2602.42</v>
       </c>
     </row>
     <row r="65">
@@ -1670,10 +1670,10 @@
         <v>8711.950000000001</v>
       </c>
       <c r="D65" t="n">
-        <v>0</v>
+        <v>1132.55</v>
       </c>
       <c r="E65" t="n">
-        <v>0</v>
+        <v>9844.5</v>
       </c>
     </row>
     <row r="66">
@@ -1689,10 +1689,10 @@
         <v>6716.12</v>
       </c>
       <c r="D66" t="n">
-        <v>0</v>
+        <v>873.1</v>
       </c>
       <c r="E66" t="n">
-        <v>0</v>
+        <v>7589.22</v>
       </c>
     </row>
     <row r="67">
@@ -1708,10 +1708,10 @@
         <v>593.22</v>
       </c>
       <c r="D67" t="n">
-        <v>0</v>
+        <v>77.12</v>
       </c>
       <c r="E67" t="n">
-        <v>0</v>
+        <v>670.34</v>
       </c>
     </row>
     <row r="68">
@@ -1727,10 +1727,10 @@
         <v>224.15</v>
       </c>
       <c r="D68" t="n">
-        <v>0</v>
+        <v>29.14</v>
       </c>
       <c r="E68" t="n">
-        <v>0</v>
+        <v>253.29</v>
       </c>
     </row>
     <row r="69">
@@ -1746,10 +1746,10 @@
         <v>169.33</v>
       </c>
       <c r="D69" t="n">
-        <v>0</v>
+        <v>22.01</v>
       </c>
       <c r="E69" t="n">
-        <v>0</v>
+        <v>191.34</v>
       </c>
     </row>
     <row r="70">
@@ -1765,10 +1765,10 @@
         <v>5285.1</v>
       </c>
       <c r="D70" t="n">
-        <v>0</v>
+        <v>687.0599999999999</v>
       </c>
       <c r="E70" t="n">
-        <v>0</v>
+        <v>5972.16</v>
       </c>
     </row>
     <row r="71">
@@ -1784,10 +1784,10 @@
         <v>343.74</v>
       </c>
       <c r="D71" t="n">
-        <v>0</v>
+        <v>44.69</v>
       </c>
       <c r="E71" t="n">
-        <v>0</v>
+        <v>388.43</v>
       </c>
     </row>
     <row r="72">
@@ -1803,10 +1803,10 @@
         <v>562.75</v>
       </c>
       <c r="D72" t="n">
-        <v>0</v>
+        <v>73.16</v>
       </c>
       <c r="E72" t="n">
-        <v>0</v>
+        <v>635.91</v>
       </c>
     </row>
     <row r="73">
@@ -1822,10 +1822,10 @@
         <v>627.27</v>
       </c>
       <c r="D73" t="n">
-        <v>0</v>
+        <v>81.55</v>
       </c>
       <c r="E73" t="n">
-        <v>0</v>
+        <v>708.8200000000001</v>
       </c>
     </row>
     <row r="74">
@@ -1841,10 +1841,10 @@
         <v>236.49</v>
       </c>
       <c r="D74" t="n">
-        <v>0</v>
+        <v>30.74</v>
       </c>
       <c r="E74" t="n">
-        <v>0</v>
+        <v>267.23</v>
       </c>
     </row>
     <row r="75">
@@ -1860,10 +1860,10 @@
         <v>856.76</v>
       </c>
       <c r="D75" t="n">
-        <v>0</v>
+        <v>111.38</v>
       </c>
       <c r="E75" t="n">
-        <v>0</v>
+        <v>968.14</v>
       </c>
     </row>
     <row r="76">
@@ -1879,10 +1879,10 @@
         <v>293.28</v>
       </c>
       <c r="D76" t="n">
-        <v>0</v>
+        <v>38.13</v>
       </c>
       <c r="E76" t="n">
-        <v>0</v>
+        <v>331.41</v>
       </c>
     </row>
     <row r="77">
@@ -1898,10 +1898,10 @@
         <v>241.85</v>
       </c>
       <c r="D77" t="n">
-        <v>0</v>
+        <v>31.44</v>
       </c>
       <c r="E77" t="n">
-        <v>0</v>
+        <v>273.29</v>
       </c>
     </row>
     <row r="78">
@@ -1917,10 +1917,10 @@
         <v>702.14</v>
       </c>
       <c r="D78" t="n">
-        <v>0</v>
+        <v>91.28</v>
       </c>
       <c r="E78" t="n">
-        <v>0</v>
+        <v>793.42</v>
       </c>
     </row>
     <row r="79">
@@ -1936,10 +1936,10 @@
         <v>422.94</v>
       </c>
       <c r="D79" t="n">
-        <v>0</v>
+        <v>54.98</v>
       </c>
       <c r="E79" t="n">
-        <v>0</v>
+        <v>477.92</v>
       </c>
     </row>
     <row r="80">
@@ -1955,10 +1955,10 @@
         <v>1.32</v>
       </c>
       <c r="D80" t="n">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="E80" t="n">
-        <v>0</v>
+        <v>1.49</v>
       </c>
     </row>
     <row r="81">
@@ -1974,10 +1974,10 @@
         <v>589.9400000000001</v>
       </c>
       <c r="D81" t="n">
-        <v>0</v>
+        <v>76.69</v>
       </c>
       <c r="E81" t="n">
-        <v>0</v>
+        <v>666.63</v>
       </c>
     </row>
     <row r="82">
@@ -1993,10 +1993,10 @@
         <v>37.38</v>
       </c>
       <c r="D82" t="n">
-        <v>0</v>
+        <v>4.86</v>
       </c>
       <c r="E82" t="n">
-        <v>0</v>
+        <v>42.24</v>
       </c>
     </row>
     <row r="83">
@@ -2012,10 +2012,10 @@
         <v>254.81</v>
       </c>
       <c r="D83" t="n">
-        <v>0</v>
+        <v>33.13</v>
       </c>
       <c r="E83" t="n">
-        <v>0</v>
+        <v>287.94</v>
       </c>
     </row>
     <row r="84">
@@ -2031,10 +2031,10 @@
         <v>8582.040000000001</v>
       </c>
       <c r="D84" t="n">
-        <v>0</v>
+        <v>1115.67</v>
       </c>
       <c r="E84" t="n">
-        <v>0</v>
+        <v>9697.709999999999</v>
       </c>
     </row>
     <row r="85">
@@ -2050,10 +2050,10 @@
         <v>721.15</v>
       </c>
       <c r="D85" t="n">
-        <v>0</v>
+        <v>93.75</v>
       </c>
       <c r="E85" t="n">
-        <v>0</v>
+        <v>814.9</v>
       </c>
     </row>
     <row r="86">
@@ -2069,10 +2069,10 @@
         <v>2534.69</v>
       </c>
       <c r="D86" t="n">
-        <v>0</v>
+        <v>329.51</v>
       </c>
       <c r="E86" t="n">
-        <v>0</v>
+        <v>2864.2</v>
       </c>
     </row>
     <row r="87">
@@ -2088,10 +2088,10 @@
         <v>975.02</v>
       </c>
       <c r="D87" t="n">
-        <v>0</v>
+        <v>126.75</v>
       </c>
       <c r="E87" t="n">
-        <v>0</v>
+        <v>1101.77</v>
       </c>
     </row>
     <row r="88">
@@ -2107,10 +2107,10 @@
         <v>38.32</v>
       </c>
       <c r="D88" t="n">
-        <v>0</v>
+        <v>4.98</v>
       </c>
       <c r="E88" t="n">
-        <v>0</v>
+        <v>43.3</v>
       </c>
     </row>
     <row r="89">
@@ -2126,10 +2126,10 @@
         <v>5016.97</v>
       </c>
       <c r="D89" t="n">
-        <v>0</v>
+        <v>652.21</v>
       </c>
       <c r="E89" t="n">
-        <v>0</v>
+        <v>5669.18</v>
       </c>
     </row>
     <row r="90">
@@ -2145,10 +2145,10 @@
         <v>5266.76</v>
       </c>
       <c r="D90" t="n">
-        <v>0</v>
+        <v>684.6799999999999</v>
       </c>
       <c r="E90" t="n">
-        <v>0</v>
+        <v>5951.44</v>
       </c>
     </row>
     <row r="91">
@@ -2164,10 +2164,10 @@
         <v>2499.72</v>
       </c>
       <c r="D91" t="n">
-        <v>0</v>
+        <v>324.96</v>
       </c>
       <c r="E91" t="n">
-        <v>0</v>
+        <v>2824.68</v>
       </c>
     </row>
     <row r="92">
@@ -2183,10 +2183,10 @@
         <v>2923.54</v>
       </c>
       <c r="D92" t="n">
-        <v>0</v>
+        <v>380.06</v>
       </c>
       <c r="E92" t="n">
-        <v>0</v>
+        <v>3303.6</v>
       </c>
     </row>
     <row r="93">
@@ -2202,10 +2202,10 @@
         <v>882.33</v>
       </c>
       <c r="D93" t="n">
-        <v>0</v>
+        <v>114.7</v>
       </c>
       <c r="E93" t="n">
-        <v>0</v>
+        <v>997.03</v>
       </c>
     </row>
     <row r="94">
@@ -2221,10 +2221,10 @@
         <v>7232.29</v>
       </c>
       <c r="D94" t="n">
-        <v>0</v>
+        <v>940.2</v>
       </c>
       <c r="E94" t="n">
-        <v>0</v>
+        <v>8172.49</v>
       </c>
     </row>
     <row r="95">
@@ -2240,10 +2240,10 @@
         <v>6606.62</v>
       </c>
       <c r="D95" t="n">
-        <v>0</v>
+        <v>858.86</v>
       </c>
       <c r="E95" t="n">
-        <v>0</v>
+        <v>7465.48</v>
       </c>
     </row>
     <row r="96">
@@ -2259,10 +2259,10 @@
         <v>552.37</v>
       </c>
       <c r="D96" t="n">
-        <v>0</v>
+        <v>71.81</v>
       </c>
       <c r="E96" t="n">
-        <v>0</v>
+        <v>624.1799999999999</v>
       </c>
     </row>
     <row r="97">
@@ -2278,10 +2278,10 @@
         <v>651.51</v>
       </c>
       <c r="D97" t="n">
-        <v>0</v>
+        <v>84.7</v>
       </c>
       <c r="E97" t="n">
-        <v>0</v>
+        <v>736.21</v>
       </c>
     </row>
     <row r="98">
@@ -2297,10 +2297,10 @@
         <v>7897.48</v>
       </c>
       <c r="D98" t="n">
-        <v>0</v>
+        <v>1026.67</v>
       </c>
       <c r="E98" t="n">
-        <v>0</v>
+        <v>8924.15</v>
       </c>
     </row>
     <row r="99">
@@ -2316,10 +2316,10 @@
         <v>642.05</v>
       </c>
       <c r="D99" t="n">
-        <v>0</v>
+        <v>83.47</v>
       </c>
       <c r="E99" t="n">
-        <v>0</v>
+        <v>725.52</v>
       </c>
     </row>
     <row r="100">
@@ -2335,10 +2335,10 @@
         <v>8298.41</v>
       </c>
       <c r="D100" t="n">
-        <v>0</v>
+        <v>1078.79</v>
       </c>
       <c r="E100" t="n">
-        <v>0</v>
+        <v>9377.200000000001</v>
       </c>
     </row>
     <row r="101">
@@ -2354,10 +2354,10 @@
         <v>657.13</v>
       </c>
       <c r="D101" t="n">
-        <v>0</v>
+        <v>85.43000000000001</v>
       </c>
       <c r="E101" t="n">
-        <v>0</v>
+        <v>742.5599999999999</v>
       </c>
     </row>
     <row r="102">
@@ -2373,10 +2373,10 @@
         <v>660.2</v>
       </c>
       <c r="D102" t="n">
-        <v>0</v>
+        <v>85.83</v>
       </c>
       <c r="E102" t="n">
-        <v>0</v>
+        <v>746.03</v>
       </c>
     </row>
     <row r="103">
@@ -2392,10 +2392,10 @@
         <v>3712.87</v>
       </c>
       <c r="D103" t="n">
-        <v>0</v>
+        <v>482.67</v>
       </c>
       <c r="E103" t="n">
-        <v>0</v>
+        <v>4195.54</v>
       </c>
     </row>
     <row r="104">
@@ -2411,10 +2411,10 @@
         <v>7733.92</v>
       </c>
       <c r="D104" t="n">
-        <v>0</v>
+        <v>1005.41</v>
       </c>
       <c r="E104" t="n">
-        <v>0</v>
+        <v>8739.33</v>
       </c>
     </row>
     <row r="105">
@@ -2430,10 +2430,10 @@
         <v>473.82</v>
       </c>
       <c r="D105" t="n">
-        <v>0</v>
+        <v>61.6</v>
       </c>
       <c r="E105" t="n">
-        <v>0</v>
+        <v>535.42</v>
       </c>
     </row>
     <row r="106">
@@ -2449,10 +2449,10 @@
         <v>621.33</v>
       </c>
       <c r="D106" t="n">
-        <v>0</v>
+        <v>80.77</v>
       </c>
       <c r="E106" t="n">
-        <v>0</v>
+        <v>702.1</v>
       </c>
     </row>
     <row r="107">
@@ -2468,10 +2468,10 @@
         <v>484.4</v>
       </c>
       <c r="D107" t="n">
-        <v>0</v>
+        <v>62.97</v>
       </c>
       <c r="E107" t="n">
-        <v>0</v>
+        <v>547.37</v>
       </c>
     </row>
     <row r="108">
@@ -2487,10 +2487,10 @@
         <v>313.78</v>
       </c>
       <c r="D108" t="n">
-        <v>0</v>
+        <v>40.79</v>
       </c>
       <c r="E108" t="n">
-        <v>0</v>
+        <v>354.57</v>
       </c>
     </row>
     <row r="109">
@@ -2506,10 +2506,10 @@
         <v>6148.43</v>
       </c>
       <c r="D109" t="n">
-        <v>0</v>
+        <v>799.3</v>
       </c>
       <c r="E109" t="n">
-        <v>0</v>
+        <v>6947.73</v>
       </c>
     </row>
     <row r="110">
@@ -2525,10 +2525,10 @@
         <v>7193.49</v>
       </c>
       <c r="D110" t="n">
-        <v>0</v>
+        <v>935.15</v>
       </c>
       <c r="E110" t="n">
-        <v>0</v>
+        <v>8128.64</v>
       </c>
     </row>
     <row r="111">
@@ -2544,10 +2544,10 @@
         <v>548.77</v>
       </c>
       <c r="D111" t="n">
-        <v>0</v>
+        <v>71.34</v>
       </c>
       <c r="E111" t="n">
-        <v>0</v>
+        <v>620.11</v>
       </c>
     </row>
     <row r="112">
@@ -2563,10 +2563,10 @@
         <v>6365.88</v>
       </c>
       <c r="D112" t="n">
-        <v>0</v>
+        <v>827.5599999999999</v>
       </c>
       <c r="E112" t="n">
-        <v>0</v>
+        <v>7193.44</v>
       </c>
     </row>
     <row r="113">
@@ -2582,10 +2582,10 @@
         <v>5578.22</v>
       </c>
       <c r="D113" t="n">
-        <v>0</v>
+        <v>725.17</v>
       </c>
       <c r="E113" t="n">
-        <v>0</v>
+        <v>6303.39</v>
       </c>
     </row>
     <row r="114">
@@ -2601,10 +2601,10 @@
         <v>661.14</v>
       </c>
       <c r="D114" t="n">
-        <v>0</v>
+        <v>85.95</v>
       </c>
       <c r="E114" t="n">
-        <v>0</v>
+        <v>747.09</v>
       </c>
     </row>
     <row r="115">
@@ -2620,10 +2620,10 @@
         <v>571.98</v>
       </c>
       <c r="D115" t="n">
-        <v>0</v>
+        <v>74.36</v>
       </c>
       <c r="E115" t="n">
-        <v>0</v>
+        <v>646.34</v>
       </c>
     </row>
     <row r="116">
@@ -2639,10 +2639,10 @@
         <v>3005.08</v>
       </c>
       <c r="D116" t="n">
-        <v>0</v>
+        <v>390.66</v>
       </c>
       <c r="E116" t="n">
-        <v>0</v>
+        <v>3395.74</v>
       </c>
     </row>
     <row r="117">
@@ -2658,10 +2658,10 @@
         <v>652.88</v>
       </c>
       <c r="D117" t="n">
-        <v>0</v>
+        <v>84.87</v>
       </c>
       <c r="E117" t="n">
-        <v>0</v>
+        <v>737.75</v>
       </c>
     </row>
     <row r="118">
@@ -2677,10 +2677,10 @@
         <v>686.83</v>
       </c>
       <c r="D118" t="n">
-        <v>0</v>
+        <v>89.29000000000001</v>
       </c>
       <c r="E118" t="n">
-        <v>0</v>
+        <v>776.12</v>
       </c>
     </row>
     <row r="119">
@@ -2696,10 +2696,10 @@
         <v>8060.31</v>
       </c>
       <c r="D119" t="n">
-        <v>0</v>
+        <v>1047.84</v>
       </c>
       <c r="E119" t="n">
-        <v>0</v>
+        <v>9108.15</v>
       </c>
     </row>
     <row r="120">
@@ -2715,10 +2715,10 @@
         <v>5622.15</v>
       </c>
       <c r="D120" t="n">
-        <v>0</v>
+        <v>730.88</v>
       </c>
       <c r="E120" t="n">
-        <v>0</v>
+        <v>6353.03</v>
       </c>
     </row>
     <row r="121">
@@ -2734,10 +2734,10 @@
         <v>6.87</v>
       </c>
       <c r="D121" t="n">
-        <v>0</v>
+        <v>0.89</v>
       </c>
       <c r="E121" t="n">
-        <v>0</v>
+        <v>7.76</v>
       </c>
     </row>
     <row r="122">
@@ -2753,10 +2753,10 @@
         <v>277.12</v>
       </c>
       <c r="D122" t="n">
-        <v>0</v>
+        <v>36.03</v>
       </c>
       <c r="E122" t="n">
-        <v>0</v>
+        <v>313.15</v>
       </c>
     </row>
     <row r="123">
@@ -2772,10 +2772,10 @@
         <v>670.23</v>
       </c>
       <c r="D123" t="n">
-        <v>0</v>
+        <v>87.13</v>
       </c>
       <c r="E123" t="n">
-        <v>0</v>
+        <v>757.36</v>
       </c>
     </row>
     <row r="124">
@@ -2791,10 +2791,10 @@
         <v>1787.59</v>
       </c>
       <c r="D124" t="n">
-        <v>0</v>
+        <v>232.39</v>
       </c>
       <c r="E124" t="n">
-        <v>0</v>
+        <v>2019.98</v>
       </c>
     </row>
     <row r="125">
@@ -2810,10 +2810,10 @@
         <v>8973.639999999999</v>
       </c>
       <c r="D125" t="n">
-        <v>0</v>
+        <v>1166.57</v>
       </c>
       <c r="E125" t="n">
-        <v>0</v>
+        <v>10140.21</v>
       </c>
     </row>
     <row r="126">
@@ -2829,10 +2829,10 @@
         <v>550.54</v>
       </c>
       <c r="D126" t="n">
-        <v>0</v>
+        <v>71.56999999999999</v>
       </c>
       <c r="E126" t="n">
-        <v>0</v>
+        <v>622.11</v>
       </c>
     </row>
     <row r="127">
@@ -2848,10 +2848,10 @@
         <v>5680.59</v>
       </c>
       <c r="D127" t="n">
-        <v>0</v>
+        <v>738.48</v>
       </c>
       <c r="E127" t="n">
-        <v>0</v>
+        <v>6419.07</v>
       </c>
     </row>
     <row r="128">
@@ -2867,10 +2867,10 @@
         <v>9488.209999999999</v>
       </c>
       <c r="D128" t="n">
-        <v>0</v>
+        <v>1233.47</v>
       </c>
       <c r="E128" t="n">
-        <v>0</v>
+        <v>10721.68</v>
       </c>
     </row>
     <row r="129">
@@ -2886,10 +2886,10 @@
         <v>841.47</v>
       </c>
       <c r="D129" t="n">
-        <v>0</v>
+        <v>109.39</v>
       </c>
       <c r="E129" t="n">
-        <v>0</v>
+        <v>950.86</v>
       </c>
     </row>
     <row r="130">
@@ -2905,10 +2905,10 @@
         <v>724.36</v>
       </c>
       <c r="D130" t="n">
-        <v>0</v>
+        <v>94.17</v>
       </c>
       <c r="E130" t="n">
-        <v>0</v>
+        <v>818.53</v>
       </c>
     </row>
     <row r="131">
@@ -2924,10 +2924,10 @@
         <v>7003</v>
       </c>
       <c r="D131" t="n">
-        <v>0</v>
+        <v>910.39</v>
       </c>
       <c r="E131" t="n">
-        <v>0</v>
+        <v>7913.39</v>
       </c>
     </row>
     <row r="132">
@@ -2943,10 +2943,10 @@
         <v>3093.65</v>
       </c>
       <c r="D132" t="n">
-        <v>0</v>
+        <v>402.17</v>
       </c>
       <c r="E132" t="n">
-        <v>0</v>
+        <v>3495.82</v>
       </c>
     </row>
     <row r="133">
@@ -2962,10 +2962,10 @@
         <v>4222.72</v>
       </c>
       <c r="D133" t="n">
-        <v>0</v>
+        <v>548.95</v>
       </c>
       <c r="E133" t="n">
-        <v>0</v>
+        <v>4771.67</v>
       </c>
     </row>
     <row r="134">
@@ -2981,10 +2981,10 @@
         <v>216.92</v>
       </c>
       <c r="D134" t="n">
-        <v>0</v>
+        <v>28.2</v>
       </c>
       <c r="E134" t="n">
-        <v>0</v>
+        <v>245.12</v>
       </c>
     </row>
     <row r="135">
@@ -3000,10 +3000,10 @@
         <v>3716.27</v>
       </c>
       <c r="D135" t="n">
-        <v>0</v>
+        <v>483.12</v>
       </c>
       <c r="E135" t="n">
-        <v>0</v>
+        <v>4199.39</v>
       </c>
     </row>
     <row r="136">
@@ -3019,10 +3019,10 @@
         <v>6744.78</v>
       </c>
       <c r="D136" t="n">
-        <v>0</v>
+        <v>876.8200000000001</v>
       </c>
       <c r="E136" t="n">
-        <v>0</v>
+        <v>7621.6</v>
       </c>
     </row>
     <row r="137">
@@ -3038,10 +3038,10 @@
         <v>3858.07</v>
       </c>
       <c r="D137" t="n">
-        <v>0</v>
+        <v>501.55</v>
       </c>
       <c r="E137" t="n">
-        <v>0</v>
+        <v>4359.62</v>
       </c>
     </row>
     <row r="138">
@@ -3057,10 +3057,10 @@
         <v>2182.28</v>
       </c>
       <c r="D138" t="n">
-        <v>0</v>
+        <v>283.7</v>
       </c>
       <c r="E138" t="n">
-        <v>0</v>
+        <v>2465.98</v>
       </c>
     </row>
     <row r="139">
@@ -3076,10 +3076,10 @@
         <v>589.83</v>
       </c>
       <c r="D139" t="n">
-        <v>0</v>
+        <v>76.68000000000001</v>
       </c>
       <c r="E139" t="n">
-        <v>0</v>
+        <v>666.51</v>
       </c>
     </row>
     <row r="140">
@@ -3095,10 +3095,10 @@
         <v>926.24</v>
       </c>
       <c r="D140" t="n">
-        <v>0</v>
+        <v>120.41</v>
       </c>
       <c r="E140" t="n">
-        <v>0</v>
+        <v>1046.65</v>
       </c>
     </row>
     <row r="141">
@@ -3114,10 +3114,10 @@
         <v>760.26</v>
       </c>
       <c r="D141" t="n">
-        <v>0</v>
+        <v>98.83</v>
       </c>
       <c r="E141" t="n">
-        <v>0</v>
+        <v>859.09</v>
       </c>
     </row>
     <row r="142">
@@ -3133,10 +3133,10 @@
         <v>3259.6</v>
       </c>
       <c r="D142" t="n">
-        <v>0</v>
+        <v>423.75</v>
       </c>
       <c r="E142" t="n">
-        <v>0</v>
+        <v>3683.35</v>
       </c>
     </row>
     <row r="143">
@@ -3152,10 +3152,10 @@
         <v>211.38</v>
       </c>
       <c r="D143" t="n">
-        <v>0</v>
+        <v>27.48</v>
       </c>
       <c r="E143" t="n">
-        <v>0</v>
+        <v>238.86</v>
       </c>
     </row>
     <row r="144">
@@ -3171,10 +3171,10 @@
         <v>5192.57</v>
       </c>
       <c r="D144" t="n">
-        <v>0</v>
+        <v>675.03</v>
       </c>
       <c r="E144" t="n">
-        <v>0</v>
+        <v>5867.6</v>
       </c>
     </row>
     <row r="145">
@@ -3190,10 +3190,10 @@
         <v>9357.98</v>
       </c>
       <c r="D145" t="n">
-        <v>0</v>
+        <v>1216.54</v>
       </c>
       <c r="E145" t="n">
-        <v>0</v>
+        <v>10574.52</v>
       </c>
     </row>
     <row r="146">
@@ -3209,10 +3209,10 @@
         <v>6542.78</v>
       </c>
       <c r="D146" t="n">
-        <v>0</v>
+        <v>850.5599999999999</v>
       </c>
       <c r="E146" t="n">
-        <v>0</v>
+        <v>7393.34</v>
       </c>
     </row>
     <row r="147">
@@ -3228,10 +3228,10 @@
         <v>542.4299999999999</v>
       </c>
       <c r="D147" t="n">
-        <v>0</v>
+        <v>70.52</v>
       </c>
       <c r="E147" t="n">
-        <v>0</v>
+        <v>612.95</v>
       </c>
     </row>
     <row r="148">
@@ -3247,10 +3247,10 @@
         <v>960.84</v>
       </c>
       <c r="D148" t="n">
-        <v>0</v>
+        <v>124.91</v>
       </c>
       <c r="E148" t="n">
-        <v>0</v>
+        <v>1085.75</v>
       </c>
     </row>
     <row r="149">
@@ -3266,10 +3266,10 @@
         <v>528.5599999999999</v>
       </c>
       <c r="D149" t="n">
-        <v>0</v>
+        <v>68.70999999999999</v>
       </c>
       <c r="E149" t="n">
-        <v>0</v>
+        <v>597.27</v>
       </c>
     </row>
     <row r="150">
@@ -3285,10 +3285,10 @@
         <v>3719.65</v>
       </c>
       <c r="D150" t="n">
-        <v>0</v>
+        <v>483.55</v>
       </c>
       <c r="E150" t="n">
-        <v>0</v>
+        <v>4203.2</v>
       </c>
     </row>
     <row r="151">
@@ -3304,10 +3304,10 @@
         <v>523.8200000000001</v>
       </c>
       <c r="D151" t="n">
-        <v>0</v>
+        <v>68.09999999999999</v>
       </c>
       <c r="E151" t="n">
-        <v>0</v>
+        <v>591.92</v>
       </c>
     </row>
     <row r="152">
@@ -3323,10 +3323,10 @@
         <v>502.08</v>
       </c>
       <c r="D152" t="n">
-        <v>0</v>
+        <v>65.27</v>
       </c>
       <c r="E152" t="n">
-        <v>0</v>
+        <v>567.35</v>
       </c>
     </row>
     <row r="153">
@@ -3342,10 +3342,10 @@
         <v>943.7</v>
       </c>
       <c r="D153" t="n">
-        <v>0</v>
+        <v>122.68</v>
       </c>
       <c r="E153" t="n">
-        <v>0</v>
+        <v>1066.38</v>
       </c>
     </row>
     <row r="154">
@@ -3361,10 +3361,10 @@
         <v>6852.46</v>
       </c>
       <c r="D154" t="n">
-        <v>0</v>
+        <v>890.8200000000001</v>
       </c>
       <c r="E154" t="n">
-        <v>0</v>
+        <v>7743.28</v>
       </c>
     </row>
     <row r="155">
@@ -3380,10 +3380,10 @@
         <v>332.19</v>
       </c>
       <c r="D155" t="n">
-        <v>0</v>
+        <v>43.18</v>
       </c>
       <c r="E155" t="n">
-        <v>0</v>
+        <v>375.37</v>
       </c>
     </row>
     <row r="156">
@@ -3399,10 +3399,10 @@
         <v>7664.21</v>
       </c>
       <c r="D156" t="n">
-        <v>0</v>
+        <v>996.35</v>
       </c>
       <c r="E156" t="n">
-        <v>0</v>
+        <v>8660.559999999999</v>
       </c>
     </row>
     <row r="157">
@@ -3418,10 +3418,10 @@
         <v>359.95</v>
       </c>
       <c r="D157" t="n">
-        <v>0</v>
+        <v>46.79</v>
       </c>
       <c r="E157" t="n">
-        <v>0</v>
+        <v>406.74</v>
       </c>
     </row>
     <row r="158">
@@ -3437,10 +3437,10 @@
         <v>8676.280000000001</v>
       </c>
       <c r="D158" t="n">
-        <v>0</v>
+        <v>1127.92</v>
       </c>
       <c r="E158" t="n">
-        <v>0</v>
+        <v>9804.200000000001</v>
       </c>
     </row>
     <row r="159">
@@ -3456,10 +3456,10 @@
         <v>784.77</v>
       </c>
       <c r="D159" t="n">
-        <v>0</v>
+        <v>102.02</v>
       </c>
       <c r="E159" t="n">
-        <v>0</v>
+        <v>886.79</v>
       </c>
     </row>
     <row r="160">
@@ -3475,10 +3475,10 @@
         <v>482.17</v>
       </c>
       <c r="D160" t="n">
-        <v>0</v>
+        <v>62.68</v>
       </c>
       <c r="E160" t="n">
-        <v>0</v>
+        <v>544.85</v>
       </c>
     </row>
     <row r="161">
@@ -3494,10 +3494,10 @@
         <v>8937.940000000001</v>
       </c>
       <c r="D161" t="n">
-        <v>0</v>
+        <v>1161.93</v>
       </c>
       <c r="E161" t="n">
-        <v>0</v>
+        <v>10099.87</v>
       </c>
     </row>
     <row r="162">
@@ -3513,10 +3513,10 @@
         <v>921.28</v>
       </c>
       <c r="D162" t="n">
-        <v>0</v>
+        <v>119.77</v>
       </c>
       <c r="E162" t="n">
-        <v>0</v>
+        <v>1041.05</v>
       </c>
     </row>
     <row r="163">
@@ -3532,10 +3532,10 @@
         <v>192.88</v>
       </c>
       <c r="D163" t="n">
-        <v>0</v>
+        <v>25.07</v>
       </c>
       <c r="E163" t="n">
-        <v>0</v>
+        <v>217.95</v>
       </c>
     </row>
     <row r="164">
@@ -3551,10 +3551,10 @@
         <v>612.96</v>
       </c>
       <c r="D164" t="n">
-        <v>0</v>
+        <v>79.68000000000001</v>
       </c>
       <c r="E164" t="n">
-        <v>0</v>
+        <v>692.64</v>
       </c>
     </row>
     <row r="165">
@@ -3570,10 +3570,10 @@
         <v>166.3</v>
       </c>
       <c r="D165" t="n">
-        <v>0</v>
+        <v>21.62</v>
       </c>
       <c r="E165" t="n">
-        <v>0</v>
+        <v>187.92</v>
       </c>
     </row>
     <row r="166">
@@ -3589,10 +3589,10 @@
         <v>4816.61</v>
       </c>
       <c r="D166" t="n">
-        <v>0</v>
+        <v>626.16</v>
       </c>
       <c r="E166" t="n">
-        <v>0</v>
+        <v>5442.77</v>
       </c>
     </row>
     <row r="167">
@@ -3608,10 +3608,10 @@
         <v>4362.94</v>
       </c>
       <c r="D167" t="n">
-        <v>0</v>
+        <v>567.1799999999999</v>
       </c>
       <c r="E167" t="n">
-        <v>0</v>
+        <v>4930.12</v>
       </c>
     </row>
     <row r="168">
@@ -3627,10 +3627,10 @@
         <v>965.3099999999999</v>
       </c>
       <c r="D168" t="n">
-        <v>0</v>
+        <v>125.49</v>
       </c>
       <c r="E168" t="n">
-        <v>0</v>
+        <v>1090.8</v>
       </c>
     </row>
     <row r="169">
@@ -3646,10 +3646,10 @@
         <v>508.9</v>
       </c>
       <c r="D169" t="n">
-        <v>0</v>
+        <v>66.16</v>
       </c>
       <c r="E169" t="n">
-        <v>0</v>
+        <v>575.0599999999999</v>
       </c>
     </row>
     <row r="170">
@@ -3665,10 +3665,10 @@
         <v>997.36</v>
       </c>
       <c r="D170" t="n">
-        <v>0</v>
+        <v>129.66</v>
       </c>
       <c r="E170" t="n">
-        <v>0</v>
+        <v>1127.02</v>
       </c>
     </row>
     <row r="171">
@@ -3684,10 +3684,10 @@
         <v>441.12</v>
       </c>
       <c r="D171" t="n">
-        <v>0</v>
+        <v>57.35</v>
       </c>
       <c r="E171" t="n">
-        <v>0</v>
+        <v>498.47</v>
       </c>
     </row>
     <row r="172">
@@ -3703,10 +3703,10 @@
         <v>4599.58</v>
       </c>
       <c r="D172" t="n">
-        <v>0</v>
+        <v>597.95</v>
       </c>
       <c r="E172" t="n">
-        <v>0</v>
+        <v>5197.53</v>
       </c>
     </row>
     <row r="173">
@@ -3722,10 +3722,10 @@
         <v>842.5599999999999</v>
       </c>
       <c r="D173" t="n">
-        <v>0</v>
+        <v>109.53</v>
       </c>
       <c r="E173" t="n">
-        <v>0</v>
+        <v>952.09</v>
       </c>
     </row>
     <row r="174">
@@ -3741,10 +3741,10 @@
         <v>9719.860000000001</v>
       </c>
       <c r="D174" t="n">
-        <v>0</v>
+        <v>1263.58</v>
       </c>
       <c r="E174" t="n">
-        <v>0</v>
+        <v>10983.44</v>
       </c>
     </row>
     <row r="175">
@@ -3760,10 +3760,10 @@
         <v>254.91</v>
       </c>
       <c r="D175" t="n">
-        <v>0</v>
+        <v>33.14</v>
       </c>
       <c r="E175" t="n">
-        <v>0</v>
+        <v>288.05</v>
       </c>
     </row>
     <row r="176">
@@ -3779,10 +3779,10 @@
         <v>2620.28</v>
       </c>
       <c r="D176" t="n">
-        <v>0</v>
+        <v>340.64</v>
       </c>
       <c r="E176" t="n">
-        <v>0</v>
+        <v>2960.92</v>
       </c>
     </row>
     <row r="177">
@@ -3798,10 +3798,10 @@
         <v>7654.15</v>
       </c>
       <c r="D177" t="n">
-        <v>0</v>
+        <v>995.04</v>
       </c>
       <c r="E177" t="n">
-        <v>0</v>
+        <v>8649.190000000001</v>
       </c>
     </row>
     <row r="178">
@@ -3817,10 +3817,10 @@
         <v>6286.32</v>
       </c>
       <c r="D178" t="n">
-        <v>0</v>
+        <v>817.22</v>
       </c>
       <c r="E178" t="n">
-        <v>0</v>
+        <v>7103.54</v>
       </c>
     </row>
     <row r="179">
@@ -3836,10 +3836,10 @@
         <v>129.34</v>
       </c>
       <c r="D179" t="n">
-        <v>0</v>
+        <v>16.81</v>
       </c>
       <c r="E179" t="n">
-        <v>0</v>
+        <v>146.15</v>
       </c>
     </row>
     <row r="180">
@@ -3855,10 +3855,10 @@
         <v>813.1</v>
       </c>
       <c r="D180" t="n">
-        <v>0</v>
+        <v>105.7</v>
       </c>
       <c r="E180" t="n">
-        <v>0</v>
+        <v>918.8</v>
       </c>
     </row>
     <row r="181">
@@ -3874,10 +3874,10 @@
         <v>8453.16</v>
       </c>
       <c r="D181" t="n">
-        <v>0</v>
+        <v>1098.91</v>
       </c>
       <c r="E181" t="n">
-        <v>0</v>
+        <v>9552.07</v>
       </c>
     </row>
     <row r="182">
@@ -3893,10 +3893,10 @@
         <v>697.1</v>
       </c>
       <c r="D182" t="n">
-        <v>0</v>
+        <v>90.62</v>
       </c>
       <c r="E182" t="n">
-        <v>0</v>
+        <v>787.72</v>
       </c>
     </row>
     <row r="183">
@@ -3912,10 +3912,10 @@
         <v>289.83</v>
       </c>
       <c r="D183" t="n">
-        <v>0</v>
+        <v>37.68</v>
       </c>
       <c r="E183" t="n">
-        <v>0</v>
+        <v>327.51</v>
       </c>
     </row>
     <row r="184">
@@ -3931,10 +3931,10 @@
         <v>3.91</v>
       </c>
       <c r="D184" t="n">
-        <v>0</v>
+        <v>0.51</v>
       </c>
       <c r="E184" t="n">
-        <v>0</v>
+        <v>4.42</v>
       </c>
     </row>
     <row r="185">
@@ -3950,10 +3950,10 @@
         <v>682.98</v>
       </c>
       <c r="D185" t="n">
-        <v>0</v>
+        <v>88.79000000000001</v>
       </c>
       <c r="E185" t="n">
-        <v>0</v>
+        <v>771.77</v>
       </c>
     </row>
     <row r="186">
@@ -3969,10 +3969,10 @@
         <v>3323.21</v>
       </c>
       <c r="D186" t="n">
-        <v>0</v>
+        <v>432.02</v>
       </c>
       <c r="E186" t="n">
-        <v>0</v>
+        <v>3755.23</v>
       </c>
     </row>
     <row r="187">
@@ -3988,10 +3988,10 @@
         <v>1.33</v>
       </c>
       <c r="D187" t="n">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="E187" t="n">
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="188">
@@ -4007,10 +4007,10 @@
         <v>236.97</v>
       </c>
       <c r="D188" t="n">
-        <v>0</v>
+        <v>30.81</v>
       </c>
       <c r="E188" t="n">
-        <v>0</v>
+        <v>267.78</v>
       </c>
     </row>
     <row r="189">
@@ -4026,10 +4026,10 @@
         <v>7769.5</v>
       </c>
       <c r="D189" t="n">
-        <v>0</v>
+        <v>1010.04</v>
       </c>
       <c r="E189" t="n">
-        <v>0</v>
+        <v>8779.540000000001</v>
       </c>
     </row>
     <row r="190">
@@ -4045,10 +4045,10 @@
         <v>720.24</v>
       </c>
       <c r="D190" t="n">
-        <v>0</v>
+        <v>93.63</v>
       </c>
       <c r="E190" t="n">
-        <v>0</v>
+        <v>813.87</v>
       </c>
     </row>
     <row r="191">
@@ -4064,10 +4064,10 @@
         <v>6883.73</v>
       </c>
       <c r="D191" t="n">
-        <v>0</v>
+        <v>894.88</v>
       </c>
       <c r="E191" t="n">
-        <v>0</v>
+        <v>7778.61</v>
       </c>
     </row>
     <row r="192">
@@ -4083,10 +4083,10 @@
         <v>474.72</v>
       </c>
       <c r="D192" t="n">
-        <v>0</v>
+        <v>61.71</v>
       </c>
       <c r="E192" t="n">
-        <v>0</v>
+        <v>536.4299999999999</v>
       </c>
     </row>
     <row r="193">
@@ -4102,10 +4102,10 @@
         <v>4611.45</v>
       </c>
       <c r="D193" t="n">
-        <v>0</v>
+        <v>599.49</v>
       </c>
       <c r="E193" t="n">
-        <v>0</v>
+        <v>5210.94</v>
       </c>
     </row>
     <row r="194">
@@ -4121,10 +4121,10 @@
         <v>921.64</v>
       </c>
       <c r="D194" t="n">
-        <v>0</v>
+        <v>119.81</v>
       </c>
       <c r="E194" t="n">
-        <v>0</v>
+        <v>1041.45</v>
       </c>
     </row>
     <row r="195">
@@ -4140,10 +4140,10 @@
         <v>212.9</v>
       </c>
       <c r="D195" t="n">
-        <v>0</v>
+        <v>27.68</v>
       </c>
       <c r="E195" t="n">
-        <v>0</v>
+        <v>240.58</v>
       </c>
     </row>
     <row r="196">
@@ -4159,10 +4159,10 @@
         <v>3167.06</v>
       </c>
       <c r="D196" t="n">
-        <v>0</v>
+        <v>411.72</v>
       </c>
       <c r="E196" t="n">
-        <v>0</v>
+        <v>3578.78</v>
       </c>
     </row>
     <row r="197">
@@ -4178,10 +4178,10 @@
         <v>3460.86</v>
       </c>
       <c r="D197" t="n">
-        <v>0</v>
+        <v>449.91</v>
       </c>
       <c r="E197" t="n">
-        <v>0</v>
+        <v>3910.77</v>
       </c>
     </row>
     <row r="198">
@@ -4197,10 +4197,10 @@
         <v>926.84</v>
       </c>
       <c r="D198" t="n">
-        <v>0</v>
+        <v>120.49</v>
       </c>
       <c r="E198" t="n">
-        <v>0</v>
+        <v>1047.33</v>
       </c>
     </row>
     <row r="199">
@@ -4216,10 +4216,10 @@
         <v>320.73</v>
       </c>
       <c r="D199" t="n">
-        <v>0</v>
+        <v>41.69</v>
       </c>
       <c r="E199" t="n">
-        <v>0</v>
+        <v>362.42</v>
       </c>
     </row>
     <row r="200">
@@ -4235,10 +4235,10 @@
         <v>751.9400000000001</v>
       </c>
       <c r="D200" t="n">
-        <v>0</v>
+        <v>97.75</v>
       </c>
       <c r="E200" t="n">
-        <v>0</v>
+        <v>849.6900000000001</v>
       </c>
     </row>
     <row r="201">
@@ -4254,10 +4254,10 @@
         <v>9197.440000000001</v>
       </c>
       <c r="D201" t="n">
-        <v>0</v>
+        <v>1195.67</v>
       </c>
       <c r="E201" t="n">
-        <v>0</v>
+        <v>10393.11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>